<commit_message>
changes to the fix
</commit_message>
<xml_diff>
--- a/tests/Behat/Resources/fixtures/countries.xlsx
+++ b/tests/Behat/Resources/fixtures/countries.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liip/Documents/acme/vendor/friendsofsylius/sylius-import-export-plugin/tests/Behat/Resources/fixtures/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6B1D23-B64B-D642-A59E-35580F712FA3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="10760" yWindow="620" windowWidth="15960" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Table 1</t>
   </si>
@@ -19,20 +28,50 @@
     <t>Code</t>
   </si>
   <si>
-    <t>DE</t>
+    <t>AD</t>
   </si>
   <si>
-    <t>CH</t>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>AX</t>
+  </si>
+  <si>
+    <t>BZ</t>
+  </si>
+  <si>
+    <t>DZ</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -44,7 +83,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -119,27 +158,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -150,25 +189,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -294,7 +393,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -303,7 +402,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -312,7 +411,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -376,8 +475,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -385,7 +484,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -393,7 +492,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -412,7 +511,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -420,7 +519,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -448,7 +547,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -474,7 +573,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -500,7 +599,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -526,7 +625,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -552,7 +651,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -578,7 +677,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +703,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -630,7 +729,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -656,7 +755,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -669,9 +768,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -688,7 +793,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -707,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -733,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -759,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -785,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -811,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -837,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -863,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,7 +1020,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +1046,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -954,9 +1059,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -970,7 +1081,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -989,7 +1100,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1130,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1156,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1182,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1208,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1123,7 +1234,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1260,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1286,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1312,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1338,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1240,54 +1351,118 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:A4"/>
+  <dimension ref="A1:IV15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.67188" style="1" customWidth="1"/>
-    <col min="2" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" style="1" customWidth="1"/>
+    <col min="2" max="256" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:1" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:1" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
+    <row r="3" spans="1:1" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="5">
+    <row r="4" spans="1:1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>